<commit_message>
cap nhat logic them lo hang bang excel va kiem tra ma sp truoc khi them lo
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_IJ\Project-LTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E7A784-DE49-4357-9F7A-ED940F7304D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79F46CE-5AE7-430E-86A6-80E624011957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11835" xr2:uid="{127CE7C5-AD73-4B95-869C-9E17D6E38290}"/>
+    <workbookView xWindow="4455" yWindow="1305" windowWidth="21600" windowHeight="11835" xr2:uid="{127CE7C5-AD73-4B95-869C-9E17D6E38290}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,33 +37,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>isDeleted</t>
+  </si>
+  <si>
+    <t>isUsed</t>
+  </si>
+  <si>
+    <t>ID sản phẩm</t>
+  </si>
+  <si>
+    <t>Số lô</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Giá gốc/sản phẩm</t>
+  </si>
+  <si>
+    <t>Ngày nhập</t>
+  </si>
+  <si>
+    <t>ID nhà cung cấp</t>
+  </si>
   <si>
     <t>productID</t>
   </si>
   <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>supplierID</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>batchNumber</t>
-  </si>
-  <si>
-    <t>importDate</t>
-  </si>
-  <si>
-    <t>createdAt</t>
-  </si>
-  <si>
-    <t>isDeleted</t>
-  </si>
-  <si>
-    <t>isUsed</t>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>productPrice</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>dimensions</t>
+  </si>
+  <si>
+    <t>CapyTech</t>
+  </si>
+  <si>
+    <t>Cam</t>
+  </si>
+  <si>
+    <t>Kim loại</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Giấy nhớ 5x</t>
+  </si>
+  <si>
+    <t>Ngày giờ tạo</t>
   </si>
 </sst>
 </file>
@@ -98,8 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,78 +456,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BE516D-A4CC-45C7-A632-5AEACAC446D0}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>30</v>
+        <v>144</v>
       </c>
       <c r="C2">
-        <v>13000</v>
+        <v>1440</v>
       </c>
       <c r="D2">
-        <v>13000</v>
+        <v>2000</v>
+      </c>
+      <c r="E2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45809</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <f ca="1">NOW()</f>
+        <v>45809.831127083336</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>31</v>
-      </c>
-      <c r="C3">
-        <v>13000</v>
-      </c>
-      <c r="D3">
-        <v>13000</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67225616-6739-46AC-9708-D16E2B71B857}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>144</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>8000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>0.9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>